<commit_message>
Updated with pressure and flow sensors
</commit_message>
<xml_diff>
--- a/Design/Concepts/ValvesAndComputer/VentilatorParts.xlsx
+++ b/Design/Concepts/ValvesAndComputer/VentilatorParts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{19834BAB-9B43-044F-9A6C-37F0144920D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CDB6E28-8313-AD49-A3DB-C866E42C539D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Prices in NZD</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Power supply</t>
+  </si>
+  <si>
+    <t>pressure sensor</t>
+  </si>
+  <si>
+    <t>flow sensor</t>
+  </si>
+  <si>
+    <t>car fuel tank pressure sensor</t>
+  </si>
+  <si>
+    <t>car mass air flow sensor</t>
   </si>
 </sst>
 </file>
@@ -558,10 +570,10 @@
   <dimension ref="B1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="17" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="17" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -739,14 +751,44 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10">
+        <v>45</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" ref="P10:P11" si="0">O10*C10</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11">
+        <v>35</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
@@ -967,7 +1009,7 @@
       </c>
       <c r="P25" s="1">
         <f>SUM(P6:P22)</f>
-        <v>780</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created 'purchased inventory'  Sheet in VentilatorParts
</commit_message>
<xml_diff>
--- a/Design/Concepts/ValvesAndComputer/VentilatorParts.xlsx
+++ b/Design/Concepts/ValvesAndComputer/VentilatorParts.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CDB6E28-8313-AD49-A3DB-C866E42C539D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{B73A4EA8-56D7-9340-A3BE-0801C5D7B74C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Purchased Inventory" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>Prices in NZD</t>
   </si>
@@ -205,13 +206,157 @@
   </si>
   <si>
     <t>car mass air flow sensor</t>
+  </si>
+  <si>
+    <t>Item Desc.</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit price </t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>SG-5010 4.8-6V Servo Motor</t>
+  </si>
+  <si>
+    <t>Jaycar</t>
+  </si>
+  <si>
+    <t>recieved</t>
+  </si>
+  <si>
+    <t>2008 MAZDA 6 AIR FLOW METER</t>
+  </si>
+  <si>
+    <t>maztech</t>
+  </si>
+  <si>
+    <t>awaiting delivery</t>
+  </si>
+  <si>
+    <t>2003 MAZDA MPV EGR VALVE</t>
+  </si>
+  <si>
+    <t>2004 MAZDA 3 AIR CLEANER BOX</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 7.9mm</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 9.5mm</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 13mm</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 16mm</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 19mm</t>
+  </si>
+  <si>
+    <t>PVC Clear Tube - 25mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Tees - 13mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Tees - 16mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Tees - 19mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Tees - 25mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Tees 4mm - 10mm - 10mm</t>
+  </si>
+  <si>
+    <t>Antelco Lateral Valves (Green Back) - 16mm</t>
+  </si>
+  <si>
+    <t>Dripline Ratchet Clip 16mm</t>
+  </si>
+  <si>
+    <t>Norma 9mm S/Steel Band Worm Drive Hose Clamps - 8mm - 12mm</t>
+  </si>
+  <si>
+    <t>Norma 9mm S/Steel Band Worm Drive Hose Clamps - 16mm - 25mm</t>
+  </si>
+  <si>
+    <t>Dripline to Lateral Reducing Joiner - 16mm/13mm</t>
+  </si>
+  <si>
+    <t>Dripline to Lateral Reducing Joiner - 19mm/16mm</t>
+  </si>
+  <si>
+    <t>Dripline to Lateral Reducing Joiner - 25mm/16mm</t>
+  </si>
+  <si>
+    <t>16mm Dripline Elbow</t>
+  </si>
+  <si>
+    <t>Lateral Inline Screen Filter - 13mm - 19mm - 16mm</t>
+  </si>
+  <si>
+    <t>50mm Plastic display side entry 8mm Pressure Gauge - 35psi 2.5Bar plastic side entry Pressure Gauge</t>
+  </si>
+  <si>
+    <t>Hansen Reducing Bush - 15mm/8mm</t>
+  </si>
+  <si>
+    <t>Antelco Female Threaded Tee - Threaded Tee - 13mm Barbs x 15mm BSPF</t>
+  </si>
+  <si>
+    <t>Antelco Female Threaded Tee - Threaded Tee - 19mm Barbs x 15mm BSPF</t>
+  </si>
+  <si>
+    <t>Antelco Female Threaded Tee - Threaded Tee - 25mm Barbs x 15mm BSPF</t>
+  </si>
+  <si>
+    <t>irrigation express</t>
+  </si>
+  <si>
+    <t>MULTICOMP HCZ-D5-A Humidity Sensor, HCZ Series, 20% to 90% RH, 5 %, Through Hole, Enclosed</t>
+  </si>
+  <si>
+    <t>OMRON 2SMPP-02 Pressure Sensor, MEMS, Air, 0 to 50°C, 37 kPa, Voltage, Gauge, Hose / Tube, 100 µA</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MC6A-7/0.2T2-PK-100M Wire, Stranded, Equipment, 7/0.2 mm Type 2, Per Metre, PVC, Pink, 0.22 mm²</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MC6A-7/0.2T2-BN-100 Wire, Stranded, Equipment, 7/0.2 mm Type 2, Per Metre, PVC, Brown, 0.22 mm²</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MC6A-7/0.2T2-YW-100 Wire, Stranded, Equipment, 7/0.2 mm Type 2, Per Metre, PVC, Yellow, 0.22 mm²</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MC6A-1/0.6T2-PK-100 Wire, Solid, Equipment, Per Metre, PVC, Pink, 23 AWG, 0.28 mm²</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MC6A-1/0.6T2-YW-100 Wire, Solid, Equipment, Per Metre, PVC, Yellow, 23 AWG, 0.28 mm²</t>
+  </si>
+  <si>
+    <t>element 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -225,16 +370,34 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF868686"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF636363"/>
+      <name val="Roboto"/>
+      <family val="18"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,16 +405,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFE5E5E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFE5E5E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFE5E5E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFE5E5E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="17" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="17" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
@@ -1025,4 +1209,799 @@
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646C272C-73BF-6743-9BD4-F5082ABF0E34}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="101.140625" customWidth="1"/>
+    <col min="3" max="4" width="15.91015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>24.9</v>
+      </c>
+      <c r="F2">
+        <f>B2*E2</f>
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>69</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F37" si="0">B3*E3</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>51.75</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1.42</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>2.98</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>3.82</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>7.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>5.68</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>18.760000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>0.33</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>0.78</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>0.45</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>0.92</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>0.92</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>2.46</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="5">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <v>0.24</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>1.9</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>1.9</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>0.47</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>0.47</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>1.08</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <v>5.19</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <v>8.5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <v>1.85</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>1.66</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30">
+        <v>1.87</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>9.98</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>19.96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <v>5.16</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>0.378</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1.8900000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>3.5599999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>